<commit_message>
data on tax credit
</commit_message>
<xml_diff>
--- a/package/calibration_data/EVrange.xlsx
+++ b/package/calibration_data/EVrange.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uab-my.sharepoint.com/personal/1621511_uab_cat/Documents/Paper_3 miquel/data_calibration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1621511\Documents_temp\Code\endogenous_innovation_and_preference_change\package\calibration_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_F25DC773A252ABDACC1048B0915A75AA5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D806F18-369D-439A-8A3B-D8698B200161}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0388A2-E86D-4310-B9E8-B2BA03CB3C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Year</t>
+    <t>EV Range (km)</t>
   </si>
   <si>
-    <t>EV Range (km)</t>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -66,8 +66,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,118 +349,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>2010</v>
+      <c r="A2" s="1">
+        <v>36526</v>
       </c>
       <c r="B2">
         <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2011</v>
+      <c r="A3" s="1">
+        <v>36892</v>
       </c>
       <c r="B3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>37257</v>
+      </c>
+      <c r="B4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>37622</v>
+      </c>
+      <c r="B5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>37987</v>
+      </c>
+      <c r="B6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>38353</v>
+      </c>
+      <c r="B7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>38718</v>
+      </c>
+      <c r="B8">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>39083</v>
+      </c>
+      <c r="B9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>39448</v>
+      </c>
+      <c r="B10">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>39814</v>
+      </c>
+      <c r="B11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>40179</v>
+      </c>
+      <c r="B12">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>40544</v>
+      </c>
+      <c r="B13">
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2012</v>
-      </c>
-      <c r="B4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>40909</v>
+      </c>
+      <c r="B14">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2013</v>
-      </c>
-      <c r="B5">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>41275</v>
+      </c>
+      <c r="B15">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>2014</v>
-      </c>
-      <c r="B6">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>41640</v>
+      </c>
+      <c r="B16">
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>2015</v>
-      </c>
-      <c r="B7">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>42005</v>
+      </c>
+      <c r="B17">
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>2016</v>
-      </c>
-      <c r="B8">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>42370</v>
+      </c>
+      <c r="B18">
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>2017</v>
-      </c>
-      <c r="B9">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>42736</v>
+      </c>
+      <c r="B19">
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>2018</v>
-      </c>
-      <c r="B10">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>43101</v>
+      </c>
+      <c r="B20">
         <v>304</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>2019</v>
-      </c>
-      <c r="B11">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B21">
         <v>336</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>2020</v>
-      </c>
-      <c r="B12">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B22">
         <v>338</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>2021</v>
-      </c>
-      <c r="B13">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B23">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B24">
         <v>349</v>
       </c>
     </row>

</xml_diff>